<commit_message>
[ver1.0] feature complete accompany.xlsx 紀錄某兩人同行機率 travel.xlsx 紀錄所有的員工
</commit_message>
<xml_diff>
--- a/accompany.xlsx
+++ b/accompany.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
   <si>
     <t>員工03</t>
   </si>
@@ -63,6 +63,33 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>70.0</t>
   </si>
 </sst>
 </file>
@@ -391,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -401,7 +428,7 @@
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="1" width="9.140625" collapsed="false"/>
+    <col min="3" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -415,91 +442,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>